<commit_message>
maj hlm + fix csl (export bib)
</commit_message>
<xml_diff>
--- a/hlm2020_nb/teach/hlm2020_nb_teach_raw.xlsx
+++ b/hlm2020_nb/teach/hlm2020_nb_teach_raw.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbr/Documents/GitHub/r-projects/hlm2020_nb/teach/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF59BF82-229C-824A-8156-8A538ED1C997}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777CD16D-9A22-4E46-B44A-BD236894E426}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>sep16_5</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>sep16_10</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>3fmhl</t>
   </si>
 </sst>
 </file>
@@ -453,11 +459,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -702,6 +708,65 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>44203.741689814815</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
+      <c r="K5">
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <v>7</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>6</v>
+      </c>
+      <c r="O5">
+        <v>7</v>
+      </c>
+      <c r="P5">
+        <v>7</v>
+      </c>
+      <c r="Q5">
+        <v>6</v>
+      </c>
+      <c r="R5">
+        <v>6</v>
+      </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>